<commit_message>
Fixed relay NC/NO pin swap issue, bumped board rev to mk1.revB
</commit_message>
<xml_diff>
--- a/pcb/eagle/PiGarage_BOM.xlsx
+++ b/pcb/eagle/PiGarage_BOM.xlsx
@@ -322,7 +322,7 @@
     <t>PiGarage mk1.revA</t>
   </si>
   <si>
-    <t>https://oshpark.com/shared_projects/ycbH6Vfq</t>
+    <t>https://oshpark.com/shared_projects/nDRBJeuH</t>
   </si>
 </sst>
 </file>
@@ -466,6 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37232,6 +37233,9 @@
     <hyperlink r:id="rId17" ref="N22"/>
     <hyperlink r:id="rId18" ref="N26"/>
   </hyperlinks>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.1" right="0.1" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>